<commit_message>
Create basic GUI without interactions, Day 16
</commit_message>
<xml_diff>
--- a/Day wise tracker.xlsx
+++ b/Day wise tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/57b5ca6df9311485/Desktop/Udemy/Python Course/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="117" documentId="8_{A48CCA7A-F28D-4CEC-8D28-556C41702FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEEC75D1-2488-4418-A0D3-204E6CACBB50}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{A48CCA7A-F28D-4CEC-8D28-556C41702FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2D4CDD4-6C9A-41AA-933F-D4C2E5864FA9}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CDE4CE16-4524-4BED-9790-32B3A6313FC0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="99">
   <si>
     <t>Python Udemy Certification</t>
   </si>
@@ -770,7 +770,7 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,6 +1075,9 @@
       <c r="D18" t="s">
         <v>67</v>
       </c>
+      <c r="E18" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">

</xml_diff>